<commit_message>
Fix all errors in test.html and add comprehensive improvements
</commit_message>
<xml_diff>
--- a/login_details.xlsx
+++ b/login_details.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,78 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-14 17:38:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-07-14 17:42:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>qw</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-07-24 21:25:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Reha_Sai</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-07-28 15:02:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>qw</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-07-28 15:26:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>qw</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-07-30 14:53:52</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>